<commit_message>
add data_cleaning for 120 to rest of the columns.
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjoshi/Documents/LendingClub/Quarterly_Loan_Stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop2\Documents\capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC8A94C-0412-4E4F-92D6-C9F10B63443B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22620" activeTab="1"/>
+    <workbookView xWindow="12000" yWindow="225" windowWidth="22020" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
     <sheet name="browseNotes" sheetId="6" r:id="rId2"/>
-    <sheet name="RejectStats" sheetId="7" r:id="rId3"/>
+    <sheet name="Full_Description" sheetId="8" r:id="rId3"/>
+    <sheet name="RejectStats" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$129</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="400">
   <si>
     <t>id</t>
   </si>
@@ -1197,12 +1205,63 @@
   <si>
     <t>The method by which the borrower receives their loan. Possible values are: CASH, DIRECT_PAY</t>
   </si>
+  <si>
+    <t xml:space="preserve">Column Names </t>
+  </si>
+  <si>
+    <t>verification_status_joint</t>
+  </si>
+  <si>
+    <t>open_il_6m</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim</t>
+  </si>
+  <si>
+    <t>revol_bal_joint</t>
+  </si>
+  <si>
+    <t>sec_app_fico_range_low</t>
+  </si>
+  <si>
+    <t>sec_app_fico_range_high</t>
+  </si>
+  <si>
+    <t>sec_app_earliest_cr_line</t>
+  </si>
+  <si>
+    <t>sec_app_inq_last_6mths</t>
+  </si>
+  <si>
+    <t>sec_app_mort_acc</t>
+  </si>
+  <si>
+    <t>sec_app_open_acc</t>
+  </si>
+  <si>
+    <t>sec_app_revol_util</t>
+  </si>
+  <si>
+    <t>sec_app_num_rev_accts</t>
+  </si>
+  <si>
+    <t>sec_app_chargeoff_within_12_mths</t>
+  </si>
+  <si>
+    <t>sec_app_collections_12_mths_ex_med</t>
+  </si>
+  <si>
+    <t>sec_app_mths_since_last_major_derog</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1383,8 +1442,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1567,6 +1632,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1818,7 +1889,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1856,6 +1927,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2250,8 +2328,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K154"/>
@@ -2261,15 +2339,15 @@
       <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="196.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>99</v>
       </c>
@@ -2277,7 +2355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>291</v>
       </c>
@@ -2286,7 +2364,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>295</v>
       </c>
@@ -2295,7 +2373,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -2304,7 +2382,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>285</v>
       </c>
@@ -2313,7 +2391,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2322,7 +2400,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -2331,7 +2409,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>252</v>
       </c>
@@ -2340,7 +2418,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>114</v>
       </c>
@@ -2349,7 +2427,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>296</v>
       </c>
@@ -2358,7 +2436,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>297</v>
       </c>
@@ -2367,7 +2445,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>105</v>
       </c>
@@ -2376,7 +2454,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>226</v>
       </c>
@@ -2385,7 +2463,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -2394,7 +2472,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2481,7 @@
       </c>
       <c r="C15" s="24"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>298</v>
       </c>
@@ -2412,7 +2490,7 @@
       </c>
       <c r="C16" s="24"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -2421,7 +2499,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2430,7 +2508,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>255</v>
       </c>
@@ -2439,7 +2517,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2448,7 +2526,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2457,7 +2535,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>166</v>
       </c>
@@ -2466,7 +2544,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2475,7 +2553,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2484,7 +2562,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2493,7 +2571,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2502,7 +2580,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -2511,7 +2589,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2520,7 +2598,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2607,7 @@
       </c>
       <c r="C29" s="24"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>277</v>
       </c>
@@ -2538,7 +2616,7 @@
       </c>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2547,7 +2625,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>287</v>
       </c>
@@ -2556,7 +2634,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>289</v>
       </c>
@@ -2565,7 +2643,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2574,7 +2652,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2583,7 +2661,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2592,7 +2670,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -2603,7 +2681,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2612,7 +2690,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2621,7 +2699,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2630,7 +2708,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2639,7 +2717,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2648,7 +2726,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2657,7 +2735,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2744,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>283</v>
       </c>
@@ -2675,7 +2753,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2687,7 +2765,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>299</v>
       </c>
@@ -2699,7 +2777,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>124</v>
       </c>
@@ -2711,7 +2789,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>125</v>
       </c>
@@ -2720,7 +2798,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>111</v>
       </c>
@@ -2729,7 +2807,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>300</v>
       </c>
@@ -2738,7 +2816,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2747,7 +2825,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>108</v>
       </c>
@@ -2756,7 +2834,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2765,7 +2843,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>273</v>
       </c>
@@ -2774,7 +2852,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>301</v>
       </c>
@@ -2783,7 +2861,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>302</v>
       </c>
@@ -2792,7 +2870,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>304</v>
       </c>
@@ -2801,7 +2879,7 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>305</v>
       </c>
@@ -2810,7 +2888,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2819,7 +2897,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>104</v>
       </c>
@@ -2828,7 +2906,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>116</v>
       </c>
@@ -2836,7 +2914,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>123</v>
       </c>
@@ -2844,7 +2922,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
@@ -2852,7 +2930,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>115</v>
       </c>
@@ -2860,7 +2938,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>122</v>
       </c>
@@ -2868,7 +2946,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>127</v>
       </c>
@@ -2876,7 +2954,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
@@ -2884,7 +2962,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>126</v>
       </c>
@@ -2892,7 +2970,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>109</v>
       </c>
@@ -2900,7 +2978,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>121</v>
       </c>
@@ -2908,7 +2986,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>120</v>
       </c>
@@ -2916,7 +2994,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>119</v>
       </c>
@@ -2926,7 +3004,7 @@
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>110</v>
       </c>
@@ -2934,7 +3012,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2942,7 +3020,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>266</v>
       </c>
@@ -2950,7 +3028,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>269</v>
       </c>
@@ -2958,7 +3036,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>271</v>
       </c>
@@ -2966,7 +3044,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>335</v>
       </c>
@@ -2974,7 +3052,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>279</v>
       </c>
@@ -2982,7 +3060,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>281</v>
       </c>
@@ -2990,7 +3068,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -2998,7 +3076,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -3006,7 +3084,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>118</v>
       </c>
@@ -3014,7 +3092,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>306</v>
       </c>
@@ -3022,7 +3100,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>129</v>
       </c>
@@ -3030,7 +3108,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
@@ -3038,7 +3116,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>103</v>
       </c>
@@ -3046,7 +3124,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>18</v>
       </c>
@@ -3054,7 +3132,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>15</v>
       </c>
@@ -3062,7 +3140,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>225</v>
       </c>
@@ -3070,7 +3148,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>31</v>
       </c>
@@ -3078,7 +3156,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>32</v>
       </c>
@@ -3086,7 +3164,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -3094,7 +3172,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>107</v>
       </c>
@@ -3102,7 +3180,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>5</v>
       </c>
@@ -3110,7 +3188,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>19</v>
       </c>
@@ -3118,7 +3196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>128</v>
       </c>
@@ -3126,7 +3204,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>113</v>
       </c>
@@ -3134,7 +3212,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>112</v>
       </c>
@@ -3142,7 +3220,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -3150,7 +3228,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>307</v>
       </c>
@@ -3158,7 +3236,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>275</v>
       </c>
@@ -3166,7 +3244,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>308</v>
       </c>
@@ -3174,7 +3252,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>293</v>
       </c>
@@ -3182,7 +3260,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>100</v>
       </c>
@@ -3190,7 +3268,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -3198,7 +3276,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -3206,7 +3284,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -3214,7 +3292,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -3222,7 +3300,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -3230,7 +3308,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>217</v>
       </c>
@@ -3238,7 +3316,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -3246,7 +3324,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>294</v>
       </c>
@@ -3254,7 +3332,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>257</v>
       </c>
@@ -3262,7 +3340,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>247</v>
       </c>
@@ -3270,7 +3348,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
         <v>310</v>
       </c>
@@ -3278,7 +3356,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
         <v>312</v>
       </c>
@@ -3286,7 +3364,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
         <v>314</v>
       </c>
@@ -3294,7 +3372,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
         <v>316</v>
       </c>
@@ -3302,7 +3380,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
         <v>318</v>
       </c>
@@ -3310,7 +3388,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
         <v>320</v>
       </c>
@@ -3318,7 +3396,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="18" t="s">
         <v>322</v>
       </c>
@@ -3326,7 +3404,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="18" t="s">
         <v>324</v>
       </c>
@@ -3334,7 +3412,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="18" t="s">
         <v>336</v>
       </c>
@@ -3342,7 +3420,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
         <v>327</v>
       </c>
@@ -3350,7 +3428,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="18" t="s">
         <v>329</v>
       </c>
@@ -3358,7 +3436,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
         <v>331</v>
       </c>
@@ -3366,7 +3444,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="18" t="s">
         <v>333</v>
       </c>
@@ -3374,7 +3452,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>347</v>
       </c>
@@ -3382,7 +3460,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>348</v>
       </c>
@@ -3390,7 +3468,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>349</v>
       </c>
@@ -3398,7 +3476,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>350</v>
       </c>
@@ -3406,7 +3484,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>351</v>
       </c>
@@ -3414,7 +3492,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>352</v>
       </c>
@@ -3422,7 +3500,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>353</v>
       </c>
@@ -3430,7 +3508,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>354</v>
       </c>
@@ -3438,7 +3516,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>355</v>
       </c>
@@ -3446,7 +3524,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>356</v>
       </c>
@@ -3454,7 +3532,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>357</v>
       </c>
@@ -3462,7 +3540,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
         <v>358</v>
       </c>
@@ -3470,7 +3548,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
         <v>359</v>
       </c>
@@ -3478,7 +3556,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
         <v>360</v>
       </c>
@@ -3486,7 +3564,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
         <v>361</v>
       </c>
@@ -3494,7 +3572,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
         <v>362</v>
       </c>
@@ -3502,7 +3580,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="9" t="s">
         <v>345</v>
       </c>
@@ -3510,7 +3588,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
         <v>346</v>
       </c>
@@ -3518,7 +3596,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
         <v>363</v>
       </c>
@@ -3526,7 +3604,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
         <v>340</v>
       </c>
@@ -3534,7 +3612,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="s">
         <v>364</v>
       </c>
@@ -3542,7 +3620,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
         <v>365</v>
       </c>
@@ -3550,7 +3628,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
         <v>366</v>
       </c>
@@ -3558,14 +3636,14 @@
         <v>344</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B154" s="13" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B129"/>
-  <sortState ref="A2:B101">
+  <autoFilter ref="A1:B129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3574,22 +3652,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="235.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="235.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>219</v>
       </c>
@@ -3597,7 +3675,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>183</v>
       </c>
@@ -3608,7 +3686,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>191</v>
       </c>
@@ -3619,7 +3697,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>192</v>
       </c>
@@ -3630,7 +3708,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>190</v>
       </c>
@@ -3641,7 +3719,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>285</v>
       </c>
@@ -3649,7 +3727,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -3659,7 +3737,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>180</v>
       </c>
@@ -3668,7 +3746,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>252</v>
       </c>
@@ -3678,7 +3756,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>114</v>
       </c>
@@ -3689,7 +3767,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>193</v>
       </c>
@@ -3700,7 +3778,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>195</v>
       </c>
@@ -3710,7 +3788,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>105</v>
       </c>
@@ -3720,7 +3798,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>106</v>
       </c>
@@ -3731,7 +3809,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>187</v>
       </c>
@@ -3742,7 +3820,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>196</v>
       </c>
@@ -3753,7 +3831,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>197</v>
       </c>
@@ -3764,7 +3842,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
@@ -3775,7 +3853,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
@@ -3784,7 +3862,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>255</v>
       </c>
@@ -3795,7 +3873,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>198</v>
       </c>
@@ -3805,7 +3883,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>239</v>
       </c>
@@ -3816,7 +3894,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>166</v>
       </c>
@@ -3827,7 +3905,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>177</v>
       </c>
@@ -3838,7 +3916,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>185</v>
       </c>
@@ -3849,7 +3927,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>173</v>
       </c>
@@ -3860,7 +3938,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>200</v>
       </c>
@@ -3871,7 +3949,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>199</v>
       </c>
@@ -3882,7 +3960,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>171</v>
       </c>
@@ -3893,7 +3971,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>8</v>
       </c>
@@ -3904,7 +3982,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>179</v>
       </c>
@@ -3915,7 +3993,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
@@ -3925,7 +4003,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>277</v>
       </c>
@@ -3935,7 +4013,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>161</v>
       </c>
@@ -3946,7 +4024,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>216</v>
       </c>
@@ -3957,7 +4035,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>287</v>
       </c>
@@ -3968,7 +4046,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>289</v>
       </c>
@@ -3979,7 +4057,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>201</v>
       </c>
@@ -3990,7 +4068,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>7</v>
       </c>
@@ -4001,7 +4079,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>172</v>
       </c>
@@ -4012,7 +4090,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -4022,7 +4100,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>186</v>
       </c>
@@ -4032,7 +4110,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>170</v>
       </c>
@@ -4042,7 +4120,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>283</v>
       </c>
@@ -4052,7 +4130,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>169</v>
       </c>
@@ -4062,7 +4140,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>124</v>
       </c>
@@ -4073,7 +4151,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>125</v>
       </c>
@@ -4083,7 +4161,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>111</v>
       </c>
@@ -4093,7 +4171,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>208</v>
       </c>
@@ -4103,7 +4181,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>160</v>
       </c>
@@ -4113,7 +4191,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>108</v>
       </c>
@@ -4123,7 +4201,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>101</v>
       </c>
@@ -4133,7 +4211,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>273</v>
       </c>
@@ -4142,7 +4220,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>202</v>
       </c>
@@ -4151,7 +4229,7 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>203</v>
       </c>
@@ -4160,7 +4238,7 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>204</v>
       </c>
@@ -4169,7 +4247,7 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>207</v>
       </c>
@@ -4178,7 +4256,7 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>205</v>
       </c>
@@ -4187,7 +4265,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>206</v>
       </c>
@@ -4196,7 +4274,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>104</v>
       </c>
@@ -4205,7 +4283,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>116</v>
       </c>
@@ -4214,7 +4292,7 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>123</v>
       </c>
@@ -4223,7 +4301,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -4232,7 +4310,7 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>115</v>
       </c>
@@ -4241,7 +4319,7 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>122</v>
       </c>
@@ -4250,7 +4328,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>127</v>
       </c>
@@ -4259,7 +4337,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>102</v>
       </c>
@@ -4268,7 +4346,7 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>126</v>
       </c>
@@ -4277,7 +4355,7 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>109</v>
       </c>
@@ -4286,7 +4364,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>121</v>
       </c>
@@ -4296,7 +4374,7 @@
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>120</v>
       </c>
@@ -4305,7 +4383,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>119</v>
       </c>
@@ -4314,7 +4392,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>110</v>
       </c>
@@ -4324,7 +4402,7 @@
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>266</v>
       </c>
@@ -4334,7 +4412,7 @@
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>269</v>
       </c>
@@ -4344,7 +4422,7 @@
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>271</v>
       </c>
@@ -4353,7 +4431,7 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>335</v>
       </c>
@@ -4362,7 +4440,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>279</v>
       </c>
@@ -4372,7 +4450,7 @@
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>281</v>
       </c>
@@ -4382,7 +4460,7 @@
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>209</v>
       </c>
@@ -4391,7 +4469,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>118</v>
       </c>
@@ -4401,7 +4479,7 @@
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>194</v>
       </c>
@@ -4411,7 +4489,7 @@
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>103</v>
       </c>
@@ -4420,7 +4498,7 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>210</v>
       </c>
@@ -4429,7 +4507,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>18</v>
       </c>
@@ -4438,7 +4516,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>189</v>
       </c>
@@ -4447,7 +4525,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>188</v>
       </c>
@@ -4456,7 +4534,7 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>212</v>
       </c>
@@ -4465,7 +4543,7 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>213</v>
       </c>
@@ -4474,7 +4552,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>174</v>
       </c>
@@ -4483,7 +4561,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>176</v>
       </c>
@@ -4493,7 +4571,7 @@
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>107</v>
       </c>
@@ -4502,7 +4580,7 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>5</v>
       </c>
@@ -4512,7 +4590,7 @@
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>19</v>
       </c>
@@ -4520,7 +4598,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>128</v>
       </c>
@@ -4528,7 +4606,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>113</v>
       </c>
@@ -4536,7 +4614,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>112</v>
       </c>
@@ -4544,7 +4622,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>275</v>
       </c>
@@ -4552,7 +4630,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>293</v>
       </c>
@@ -4560,7 +4638,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>100</v>
       </c>
@@ -4568,15 +4646,15 @@
         <v>157</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>217</v>
+        <v>399</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>215</v>
       </c>
@@ -4584,7 +4662,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>211</v>
       </c>
@@ -4592,7 +4670,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>214</v>
       </c>
@@ -4600,7 +4678,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>16</v>
       </c>
@@ -4608,7 +4686,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>257</v>
       </c>
@@ -4616,7 +4694,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>247</v>
       </c>
@@ -4624,71 +4702,71 @@
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
-        <v>310</v>
+        <v>387</v>
       </c>
       <c r="B108" s="18" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>312</v>
+        <v>388</v>
       </c>
       <c r="B109" s="18" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>314</v>
+        <v>389</v>
       </c>
       <c r="B110" s="18" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>316</v>
+        <v>390</v>
       </c>
       <c r="B111" s="18" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>318</v>
+        <v>391</v>
       </c>
       <c r="B112" s="18" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>320</v>
+        <v>392</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>322</v>
+        <v>393</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>324</v>
+        <v>394</v>
       </c>
       <c r="B115" s="18" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>336</v>
       </c>
@@ -4696,39 +4774,39 @@
         <v>326</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
-        <v>327</v>
+        <v>395</v>
       </c>
       <c r="B117" s="18" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
-        <v>329</v>
+        <v>396</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
-        <v>331</v>
+        <v>397</v>
       </c>
       <c r="B119" s="18" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
-        <v>333</v>
+        <v>398</v>
       </c>
       <c r="B120" s="18" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>362</v>
       </c>
@@ -4736,18 +4814,18 @@
         <v>382</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B123" s="13" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B89">
-    <sortState ref="A2:B107">
+  <autoFilter ref="A1:B89" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B107">
       <sortCondition ref="A1:A107"/>
     </sortState>
   </autoFilter>
-  <sortState ref="D2:D93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D93">
     <sortCondition ref="D53:D144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4756,20 +4834,903 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD42FC05-CD30-4BD7-9459-131C8604EDA0}">
+  <dimension ref="A1:B147"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="124" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="25" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="25" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="25" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="25" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="B116" t="str">
+        <f>VLOOKUP(A116,LoanStats!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Credit inquiries in the last 6 months at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="B117" t="str">
+        <f>VLOOKUP(A117,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Number of mortgage accounts at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="B118" t="str">
+        <f>VLOOKUP(A118,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Number of open trades at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="B119" t="str">
+        <f>VLOOKUP(A119,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Ratio of total current balance to high credit/credit limit for all revolving accounts</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="B120" t="str">
+        <f>VLOOKUP(A120,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Number of currently active installment trades at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="B121" t="str">
+        <f>VLOOKUP(A121,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Number of revolving accounts at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="B122" t="str">
+        <f>VLOOKUP(A122,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Number of charge-offs within last 12 months at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="B123" t="str">
+        <f>VLOOKUP(A123,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Number of collections within last 12 months excluding medical collections at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="B124" t="str">
+        <f>VLOOKUP(A124,browseNotes!A:B,2,FALSE)</f>
+        <v xml:space="preserve"> Months since most recent 90-day or worse rating at time of application for the secondary applicant</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="B125" t="str">
+        <f>VLOOKUP(A125,LoanStats!A:B,2,FALSE)</f>
+        <v>Flags whether or not the borrower is on a hardship plan</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="B126" t="str">
+        <f>VLOOKUP(A126,LoanStats!A:B,2,FALSE)</f>
+        <v>Describes the hardship plan offering</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B127" t="str">
+        <f>VLOOKUP(A127,LoanStats!A:B,2,FALSE)</f>
+        <v>Describes the reason the hardship plan was offered</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="B128" t="str">
+        <f>VLOOKUP(A128,LoanStats!A:B,2,FALSE)</f>
+        <v>Describes if the hardship plan is active, pending, canceled, completed, or broken</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="B129" t="str">
+        <f>VLOOKUP(A129,LoanStats!A:B,2,FALSE)</f>
+        <v>Amount of months that the borrower is expected to pay less than the contractual monthly payment amount due to a hardship plan</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="B130" t="str">
+        <f>VLOOKUP(A130,LoanStats!A:B,2,FALSE)</f>
+        <v>The interest payment that the borrower has committed to make each month while they are on a hardship plan</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="B131" t="str">
+        <f>VLOOKUP(A131,LoanStats!A:B,2,FALSE)</f>
+        <v>The start date of the hardship plan period</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="B132" t="str">
+        <f>VLOOKUP(A132,LoanStats!A:B,2,FALSE)</f>
+        <v>The end date of the hardship plan period</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="B133" t="str">
+        <f>VLOOKUP(A133,LoanStats!A:B,2,FALSE)</f>
+        <v>The day the first hardship plan payment is due. For example, if a borrower has a hardship plan period of 3 months, the start date is the start of the three-month period in which the borrower is allowed to make interest-only payments.</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="B134" t="str">
+        <f>VLOOKUP(A134,LoanStats!A:B,2,FALSE)</f>
+        <v>The number of months the borrower will make smaller payments than normally obligated due to a hardship plan</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="B135" t="str">
+        <f>VLOOKUP(A135,LoanStats!A:B,2,FALSE)</f>
+        <v>Account days past due as of the hardship plan start date</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="B136" t="str">
+        <f>VLOOKUP(A136,LoanStats!A:B,2,FALSE)</f>
+        <v>Loan Status as of the hardship plan start date</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="B137" t="str">
+        <f>VLOOKUP(A137,LoanStats!A:B,2,FALSE)</f>
+        <v>The original projected additional interest amount that will accrue for the given hardship payment plan as of the Hardship Start Date. This field will be null if the borrower has broken their hardship payment plan.</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="B138" t="str">
+        <f>VLOOKUP(A138,LoanStats!A:B,2,FALSE)</f>
+        <v>The payoff balance amount as of the hardship plan start date</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="B139" t="str">
+        <f>VLOOKUP(A139,LoanStats!A:B,2,FALSE)</f>
+        <v>The last payment amount as of the hardship plan start date</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="B140" t="str">
+        <f>VLOOKUP(A140,LoanStats!A:B,2,FALSE)</f>
+        <v>The method by which the borrower receives their loan. Possible values are: CASH, DIRECT_PAY</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="B141" t="str">
+        <f>VLOOKUP(A141,LoanStats!A:B,2,FALSE)</f>
+        <v>Flags whether or not the borrower, who has charged-off, is working with a debt-settlement company.</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="B142" t="str">
+        <f>VLOOKUP(A142,LoanStats!A:B,2,FALSE)</f>
+        <v>The most recent date that the Debt_Settlement_Flag has been set  </v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="B143" t="str">
+        <f>VLOOKUP(A143,LoanStats!A:B,2,FALSE)</f>
+        <v>The status of the borrower’s settlement plan. Possible values are: COMPLETE, ACTIVE, BROKEN, CANCELLED, DENIED, DRAFT</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="B144" t="str">
+        <f>VLOOKUP(A144,LoanStats!A:B,2,FALSE)</f>
+        <v>The date that the borrower agrees to the settlement plan</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="B145" t="str">
+        <f>VLOOKUP(A145,LoanStats!A:B,2,FALSE)</f>
+        <v>The loan amount that the borrower has agreed to settle for</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="B146" t="str">
+        <f>VLOOKUP(A146,LoanStats!A:B,2,FALSE)</f>
+        <v>The settlement amount as a percentage of the payoff balance amount on the loan</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="B147" t="str">
+        <f>VLOOKUP(A147,LoanStats!A:B,2,FALSE)</f>
+        <v>The number of months that the borrower will be on the settlement plan</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>227</v>
       </c>
@@ -4777,7 +5738,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>228</v>
       </c>
@@ -4785,7 +5746,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>229</v>
       </c>
@@ -4793,7 +5754,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>230</v>
       </c>
@@ -4801,7 +5762,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>243</v>
       </c>
@@ -4809,7 +5770,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>231</v>
       </c>
@@ -4817,7 +5778,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>245</v>
       </c>
@@ -4825,7 +5786,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>232</v>
       </c>
@@ -4833,7 +5794,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>233</v>
       </c>
@@ -4841,7 +5802,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>234</v>
       </c>
@@ -4849,16 +5810,16 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10"/>
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>

</xml_diff>